<commit_message>
* fixed wrong estimate in maternityLeave86.xlsx file. Somehow the same estimate from maternityLeave79 was in maternityLeave86.xlsx. However, the difference between the two estimates is marginal. * Changed entitlement period of "Erziehungsgeld" to from 8 to 10 months. 8 months is the correct value, as during the first two months a different benefit is payed, which remained unchanged the entire time. Even pre 1979
</commit_message>
<xml_diff>
--- a/estimates/maternityLeave86.xlsx
+++ b/estimates/maternityLeave86.xlsx
@@ -982,10 +982,10 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>-6.9999999999999999E-4</v>
+        <v>-5.9999999999999995E-4</v>
       </c>
       <c r="C3">
-        <v>1.6000000000000001E-3</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="J3">
         <v>2</v>

</xml_diff>